<commit_message>
Merge di due linked list ordinate e tenere l'ordine
Scorrimento in parallelo
</commit_message>
<xml_diff>
--- a/spiegazioni/esercizi.xlsx
+++ b/spiegazioni/esercizi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wissel\OneDrive\Desktop\leetcode_solutions\spiegazioni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FF133D-204D-4583-AD8D-7E984CF76A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F463EC-6D82-4C03-AFEC-8178DC1C86D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Struttura dati</t>
   </si>
@@ -67,6 +67,30 @@
   </si>
   <si>
     <t>medio</t>
+  </si>
+  <si>
+    <t>mediani di due array ordinati</t>
+  </si>
+  <si>
+    <t>creo la somma dei due array, la sorto e analizzo la sua dimensione: se pari, prendo i valori ris[len(ris)//2] e ris[len(ris//2)-1 e ne faccio la media; se dispari, prendo solo il primo</t>
+  </si>
+  <si>
+    <t>O(log (n+m)</t>
+  </si>
+  <si>
+    <t>difficile</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>merg di due linked list ordinate</t>
+  </si>
+  <si>
+    <t>itero in parallelo in entrambe e metto il valore minimo</t>
+  </si>
+  <si>
+    <t>O(min(m,n))\</t>
   </si>
 </sst>
 </file>
@@ -413,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,6 +503,40 @@
         <v>13</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
sub-stringa palindroma più grande
Si analizza ogni carattere come se fosse il centro della sub-stringa, si analizzano i caratteri nell'intrno e si verifica che sia palindroma
</commit_message>
<xml_diff>
--- a/spiegazioni/esercizi.xlsx
+++ b/spiegazioni/esercizi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wissel\OneDrive\Desktop\leetcode_solutions\spiegazioni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F463EC-6D82-4C03-AFEC-8178DC1C86D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D20871D-3555-4F68-903A-7ECE40DB855A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Struttura dati</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>O(min(m,n))\</t>
+  </si>
+  <si>
+    <t>Array di Linked List</t>
+  </si>
+  <si>
+    <t>merge di k linked list orinate</t>
+  </si>
+  <si>
+    <t>creo una mappa con key=valore nodo value=numero occorrenze, iterando per tutte le linke list. Una volta creata la mappa, la ordino mediante tuple e liste e cro k nodi relativi ad una entry quanto è il valore dell'occorrenza.</t>
+  </si>
+  <si>
+    <t>O(n^2)</t>
   </si>
 </sst>
 </file>
@@ -113,7 +125,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,6 +135,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -154,9 +172,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -437,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,7 +488,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -479,14 +498,14 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -496,14 +515,14 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -513,14 +532,14 @@
       <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -530,13 +549,33 @@
       <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Esercizi 9-7 di leetcode (palyndrom integer ed invert integer)
</commit_message>
<xml_diff>
--- a/spiegazioni/esercizi.xlsx
+++ b/spiegazioni/esercizi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wissel\OneDrive\Desktop\leetcode_solutions\spiegazioni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC8A544-7858-460C-AACE-AA082092D42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B090014B-13A8-4962-82B6-BA69F9FAB101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>Struttura dati</t>
   </si>
@@ -112,6 +112,21 @@
   </si>
   <si>
     <t>O(min(m,n))</t>
+  </si>
+  <si>
+    <t>Interi</t>
+  </si>
+  <si>
+    <t>inverti un intero (return 0 se è un intero non rappresentato da 32 bit</t>
+  </si>
+  <si>
+    <t>trasforma l'intero in stringa; verifica la negatività. Se negativo, memorizza la negatività e splitta la stringa da 1 a n. Da n-1 fino a 0 int*10**j</t>
+  </si>
+  <si>
+    <t>Vedi se un numero è palindromo</t>
+  </si>
+  <si>
+    <t>1.come esercizio (inverti numero): 2. come vede se ima stringa è palindroma</t>
   </si>
 </sst>
 </file>
@@ -134,7 +149,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,6 +183,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -210,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -218,6 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -501,14 +523,14 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.6640625" customWidth="1"/>
     <col min="2" max="2" width="45.44140625" customWidth="1"/>
-    <col min="3" max="3" width="45.21875" customWidth="1"/>
+    <col min="3" max="3" width="49.88671875" customWidth="1"/>
     <col min="4" max="4" width="34.77734375" customWidth="1"/>
     <col min="5" max="5" width="29.44140625" customWidth="1"/>
   </cols>
@@ -632,8 +654,40 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>